<commit_message>
New UniTemp Updates from quen0n
</commit_message>
<xml_diff>
--- a/applications/plugins/unitemp/sensors/Sensors.xlsx
+++ b/applications/plugins/unitemp/sensors/Sensors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quenon\Desktop\unleashed-firmware\applications\plugins\unitemp_flipperzero\sensors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AA3276-7F2D-47DB-8760-8FA46B76DC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27ABB0A4-1E47-48C4-A260-10BD339178F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{24761252-9F86-4A6F-8BB6-52E17BE4300A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="81">
   <si>
     <t>Temperature</t>
   </si>
@@ -427,6 +427,15 @@
   </si>
   <si>
     <t>-40…125 °C</t>
+  </si>
+  <si>
+    <t>BMP180</t>
+  </si>
+  <si>
+    <t>1.8...3.6V</t>
+  </si>
+  <si>
+    <t>0.01 hPa</t>
   </si>
 </sst>
 </file>
@@ -839,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30197D5-1B8F-46B2-AB75-05B6E656A3AB}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,10 +1339,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>17</v>
@@ -1345,7 +1354,7 @@
         <v>35</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -1357,12 +1366,12 @@
         <v>27</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>62</v>
@@ -1379,15 +1388,9 @@
       <c r="F17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
       <c r="J17" s="3" t="s">
         <v>50</v>
       </c>
@@ -1400,33 +1403,45 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>63</v>
@@ -1441,7 +1456,7 @@
         <v>32</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -1452,7 +1467,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>63</v>
@@ -1464,10 +1479,10 @@
         <v>47</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -1475,6 +1490,32 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>